<commit_message>
updated bug metrics with json bugs
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Function</t>
   </si>
@@ -72,10 +72,19 @@
     <t>Issue</t>
   </si>
   <si>
-    <t>#1</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Heatmap</t>
+  </si>
+  <si>
+    <t>Jsons</t>
+  </si>
+  <si>
+    <t>Jsons ordering unable to suit to wiki's requirements</t>
+  </si>
+  <si>
+    <t>semanticplacein json output  not sorted</t>
   </si>
 </sst>
 </file>
@@ -305,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -338,9 +347,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -711,13 +717,13 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="46.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
@@ -751,8 +757,8 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>17</v>
+      <c r="A2" s="8">
+        <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>6</v>
@@ -769,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>11</v>
@@ -785,13 +791,29 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>11</v>
+      </c>
       <c r="H3" s="14" t="s">
         <v>12</v>
       </c>
@@ -803,13 +825,29 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A4" s="27"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="16" t="s">
         <v>13</v>
       </c>
@@ -823,9 +861,9 @@
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="18"/>
       <c r="C5" s="28"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="J5" s="19"/>
@@ -833,9 +871,9 @@
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="18"/>
       <c r="C6" s="28"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="20"/>
       <c r="H6" s="19" t="s">
         <v>14</v>
@@ -851,102 +889,102 @@
     <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="18"/>
       <c r="C7" s="28"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="18"/>
       <c r="C8" s="28"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="18"/>
       <c r="C9" s="28"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="18"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="18"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="18"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="18"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Updated bug metrics with bootstrap and ui bugs
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Function</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>semanticplacein json output  not sorted</t>
+  </si>
+  <si>
+    <t>Bootstrap is unable to insert special characters</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>UI - Links</t>
+  </si>
+  <si>
+    <t>Broken links</t>
   </si>
 </sst>
 </file>
@@ -717,7 +729,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -767,11 +779,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="11">
-        <f t="shared" ref="D2:D4" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
+        <f t="shared" ref="D2:D6" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="E2" s="12">
-        <f t="shared" ref="E2:E4" si="1">IF(G2 = "Y",0,D2)</f>
+        <f t="shared" ref="E2:E6" si="1">IF(G2 = "Y",0,D2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -859,28 +871,62 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="20"/>
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="H5" s="21"/>
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A6" s="18"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="20"/>
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="H6" s="19" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="22">
         <f>SUM(E:E)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Edited Bug metrics with new issues logged in GITLAB
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-PC\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metrics" sheetId="1" r:id="rId1"/>
+    <sheet name="Guidelines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Function</t>
   </si>
@@ -97,13 +103,43 @@
   </si>
   <si>
     <t>Broken links</t>
+  </si>
+  <si>
+    <t>Low Impact (1 points)</t>
+  </si>
+  <si>
+    <t>Unimportant. Typo error or small user interface alignment issues.</t>
+  </si>
+  <si>
+    <t>High Impact (5 points)</t>
+  </si>
+  <si>
+    <t>The system runs. However, some non-critical functionalities are not working.</t>
+  </si>
+  <si>
+    <t>Critical Impact(10 points)</t>
+  </si>
+  <si>
+    <t>The system is down or is un-usable after a short period of time. We have to fix the bugs to continue.</t>
+  </si>
+  <si>
+    <t>OpenShift-Bootstrap</t>
+  </si>
+  <si>
+    <t>OpenShift-Heatmap</t>
+  </si>
+  <si>
+    <t>appusage table and locationusage table not found; causes system to crash when initializing bootstrap. table name is caps Sensitive. need to rename in IDE.</t>
+  </si>
+  <si>
+    <t>System crashes when heatmap request was sent. Possibly table name (appusage and locationusage) needs to be renamed (case sensitive)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -113,32 +149,57 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF999999"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +230,20 @@
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -322,11 +395,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -366,6 +529,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,6 +588,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -729,18 +924,21 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="46.81640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -768,7 +966,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -779,11 +977,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="11">
-        <f t="shared" ref="D2:D6" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
+        <f t="shared" ref="D2:D8" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
         <v>10</v>
       </c>
       <c r="E2" s="12">
-        <f t="shared" ref="E2:E6" si="1">IF(G2 = "Y",0,D2)</f>
+        <f t="shared" ref="E2:E8" si="1">IF(G2 = "Y",0,D2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -802,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27">
         <v>2</v>
       </c>
@@ -836,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27">
         <v>3</v>
       </c>
@@ -870,7 +1068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -878,15 +1076,15 @@
         <v>6</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5" s="34" t="s">
         <v>22</v>
@@ -897,7 +1095,7 @@
       <c r="H5" s="21"/>
       <c r="J5" s="19"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18">
         <v>5</v>
       </c>
@@ -926,29 +1124,63 @@
       </c>
       <c r="I6" s="22">
         <f>SUM(E:E)</f>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J6" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A8" s="18"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="23"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1">
+    <row r="7" spans="1:10" ht="61" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
       <c r="C9" s="28"/>
       <c r="D9" s="33"/>
@@ -956,7 +1188,7 @@
       <c r="F9" s="34"/>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="19"/>
       <c r="C10" s="33"/>
@@ -965,7 +1197,7 @@
       <c r="F10" s="34"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
       <c r="C11" s="33"/>
@@ -974,7 +1206,7 @@
       <c r="F11" s="34"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
       <c r="C12" s="33"/>
@@ -983,7 +1215,7 @@
       <c r="F12" s="34"/>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="33"/>
@@ -992,7 +1224,7 @@
       <c r="F13" s="34"/>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="19"/>
       <c r="C14" s="33"/>
@@ -1001,7 +1233,7 @@
       <c r="F14" s="34"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="C15" s="33"/>
       <c r="D15" s="34"/>
@@ -1009,7 +1241,7 @@
       <c r="F15" s="34"/>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="C16" s="33"/>
       <c r="D16" s="34"/>
@@ -1017,7 +1249,7 @@
       <c r="F16" s="34"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
@@ -1025,7 +1257,7 @@
       <c r="F17" s="34"/>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
@@ -1033,11 +1265,11 @@
       <c r="F18" s="34"/>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -1064,4 +1296,56 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
+    <col min="2" max="2" width="141.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created test cases for Add Batch Updated Bug metrics Updated Presentation for Supervisor Meeting with bug Metrics
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="11835" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="77">
   <si>
     <t>Function</t>
   </si>
@@ -84,13 +84,7 @@
     <t>Heatmap</t>
   </si>
   <si>
-    <t>Jsons</t>
-  </si>
-  <si>
     <t>Jsons ordering unable to suit to wiki's requirements</t>
-  </si>
-  <si>
-    <t>semanticplacein json output  not sorted</t>
   </si>
   <si>
     <t>Bootstrap is unable to insert special characters</t>
@@ -146,6 +140,123 @@
   <si>
     <t>Bad Gateway:The proxy server received an invalid response from an upstream server.
 System unable to load a big zip file. (Might need to increase session time.)</t>
+  </si>
+  <si>
+    <t>Openshift - Test case Fail</t>
+  </si>
+  <si>
+    <t>Error Messages for Location.csv and Location-Lookup don't tally</t>
+  </si>
+  <si>
+    <t>Openshift - Error messages not in sequence</t>
+  </si>
+  <si>
+    <t>The Error messages are not printed in the right order. Eg. Row 21 appears before row 10.</t>
+  </si>
+  <si>
+    <t>Bootstrap - Cannot load large data file (Data-zip 1)</t>
+  </si>
+  <si>
+    <t>The first data file of thousand entries cannot load finish before Java throws a Java Heap/Java out of memory error</t>
+  </si>
+  <si>
+    <t>Bootstrap - Cannot load large data file (Data-zip 3)</t>
+  </si>
+  <si>
+    <t>The third data file of a million entries cannot load finish before Java throws a Java Heap/Java out of memory error</t>
+  </si>
+  <si>
+    <t>Bootstrap - Duplicate entry rows are not returning</t>
+  </si>
+  <si>
+    <t>Duplicates in Bootstrap for the "most recent entry" have been solved, but then checking with the database for AddBatch are not displaying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartphone usage heatmap - misread instructions </t>
+  </si>
+  <si>
+    <t>Usage heatmap not supposed to take location data as "not there" after 5 minutes.</t>
+  </si>
+  <si>
+    <t>Bootstrap - Add Batch</t>
+  </si>
+  <si>
+    <t>Bootstrap - Main Function</t>
+  </si>
+  <si>
+    <t>Bootstrap - JSON Token</t>
+  </si>
+  <si>
+    <t>Bootstrap JSON does not load. Token is not passing through properly. Always returns error</t>
+  </si>
+  <si>
+    <t>Testing of Function</t>
+  </si>
+  <si>
+    <t>After logging out, database refreshes</t>
+  </si>
+  <si>
+    <t>Login - Database</t>
+  </si>
+  <si>
+    <t>After start-up, the program does not allow entry because values not in database</t>
+  </si>
+  <si>
+    <t>Login - Values</t>
+  </si>
+  <si>
+    <t>JSONs</t>
+  </si>
+  <si>
+    <t>Error Messages passing to the UI cannot be resused for the JSON. Therefore, the controller is not that helpful</t>
+  </si>
+  <si>
+    <t>semanticplace in json output not sorted</t>
+  </si>
+  <si>
+    <t>Delete Location - UI</t>
+  </si>
+  <si>
+    <t>Delete Location UI not displaying properly</t>
+  </si>
+  <si>
+    <t>Delete Location</t>
+  </si>
+  <si>
+    <t>Delete Location Test</t>
+  </si>
+  <si>
+    <t>Delete Location - Logic</t>
+  </si>
+  <si>
+    <t>Delete Location (Choosing Options) don't delete the right choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap </t>
+  </si>
+  <si>
+    <t>Does not consider test case of no file uploaded</t>
+  </si>
+  <si>
+    <t>Delete Location - Values</t>
+  </si>
+  <si>
+    <t>Delete Location does not consider taking no values</t>
+  </si>
+  <si>
+    <t>Add Batch</t>
+  </si>
+  <si>
+    <t>Cannot read any number of files</t>
+  </si>
+  <si>
+    <t>Fails Test case for App.csv</t>
+  </si>
+  <si>
+    <t>Checking of date allows dates that have an inverted date format eg. DD/MM/YYYY instead of YYYY/MM/DD</t>
+  </si>
+  <si>
+    <t>Categories are loaded in DAOs. Need to keep instantiating DAOs in reports.</t>
   </si>
 </sst>
 </file>
@@ -508,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -517,37 +628,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
@@ -572,8 +659,80 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -988,350 +1147,752 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11">
-        <f t="shared" ref="D2:D10" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
-        <v>10</v>
-      </c>
-      <c r="E2" s="12">
-        <f t="shared" ref="E2:E10" si="1">IF(G2 = "Y",0,D2)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="D2" s="26">
+        <f t="shared" ref="D2:D13" si="0">VLOOKUP(C2,$I$2:$J$5,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="E2" s="27">
+        <f t="shared" ref="E2:E30" si="1">IF(G2 = "Y",0,D2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="14" t="s">
+      <c r="G2" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27">
+      <c r="A3" s="29">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E3" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="E3" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27">
+      <c r="A4" s="29">
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="29" t="s">
+      <c r="B4" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E4" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="E4" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+      <c r="A5" s="33">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E5" s="12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F5" s="34" t="s">
+      <c r="E5" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="33">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E6" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="19" t="s">
+      <c r="E6" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="14">
         <f>SUM(E:E)</f>
         <v>11</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18">
+      <c r="A7" s="33">
         <v>6</v>
       </c>
-      <c r="B7" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11">
+      <c r="B7" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E7" s="12">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>23</v>
+      <c r="E7" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18">
+      <c r="A8" s="33">
         <v>7</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="B8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E8" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="41" t="s">
+      <c r="E8" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
-        <v>8</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E9" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="20" t="s">
+      <c r="E9" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18">
+      <c r="A10" s="33">
         <v>9</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="B10" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="26">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="27">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33">
+        <v>10</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G11" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33">
+        <v>11</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33">
+        <v>12</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="43">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="33">
+        <v>13</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="43">
+        <v>10</v>
+      </c>
+      <c r="E14" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="33">
+        <v>14</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="43">
+        <v>5</v>
+      </c>
+      <c r="E15" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="33">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="43">
+        <v>10</v>
+      </c>
+      <c r="E16" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="33">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="43">
+        <v>5</v>
+      </c>
+      <c r="E17" s="35">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="33">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="43">
+        <v>5</v>
+      </c>
+      <c r="E18" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="33">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="45">
+        <v>5</v>
+      </c>
+      <c r="E19" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="40">
+        <v>19</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="46">
+        <v>10</v>
+      </c>
+      <c r="E20" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>20</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="45">
+        <v>1</v>
+      </c>
+      <c r="E21" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
+        <v>21</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="45">
+        <v>1</v>
+      </c>
+      <c r="E22" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>22</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="45">
+        <v>1</v>
+      </c>
+      <c r="E23" s="35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26"/>
+      <c r="B24" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="45">
+        <v>5</v>
+      </c>
+      <c r="E24" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29">
+        <v>24</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="45">
+        <v>5</v>
+      </c>
+      <c r="E25" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>25</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="45">
+        <v>5</v>
+      </c>
+      <c r="E26" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>26</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="45">
+        <v>5</v>
+      </c>
+      <c r="E27" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="29">
+        <v>27</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="45">
+        <v>10</v>
+      </c>
+      <c r="E28" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="45">
+        <v>10</v>
+      </c>
+      <c r="E29" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="29">
+        <v>29</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="45">
+        <v>10</v>
+      </c>
+      <c r="E30" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" s="47" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I6">
@@ -1345,6 +1906,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1368,35 +1930,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B3" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B4" s="20" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Presentation to latest amendment and the Bug Metrics
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="11840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="11835" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Guidelines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1100,21 +1105,21 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="46.83203125" customWidth="1"/>
-    <col min="8" max="8" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1142,7 +1147,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="32.25" customHeight="1">
+    <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -1176,7 +1181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -1210,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -1244,7 +1249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -1271,7 +1276,7 @@
       <c r="H5" s="13"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -1306,7 +1311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="61" customHeight="1">
+    <row r="7" spans="1:10" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -1331,7 +1336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" customHeight="1">
+    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="33">
         <v>7</v>
       </c>
@@ -1356,7 +1361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="42.5" customHeight="1">
+    <row r="9" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33">
         <v>8</v>
       </c>
@@ -1381,7 +1386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="65.5" customHeight="1">
+    <row r="10" spans="1:10" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="33">
         <v>9</v>
       </c>
@@ -1406,7 +1411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="33">
         <v>10</v>
       </c>
@@ -1431,7 +1436,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="48.75" customHeight="1">
+    <row r="12" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="33">
         <v>11</v>
       </c>
@@ -1456,7 +1461,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="54" customHeight="1">
+    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33">
         <v>12</v>
       </c>
@@ -1481,7 +1486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="54.75" customHeight="1">
+    <row r="14" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1505,7 +1510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" customHeight="1">
+    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="33">
         <v>14</v>
       </c>
@@ -1529,7 +1534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="49.5" customHeight="1">
+    <row r="16" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33">
         <v>15</v>
       </c>
@@ -1553,7 +1558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33">
         <v>16</v>
       </c>
@@ -1577,7 +1582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1">
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="33">
         <v>17</v>
       </c>
@@ -1601,7 +1606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1">
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33">
         <v>18</v>
       </c>
@@ -1625,7 +1630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1">
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="40">
         <v>19</v>
       </c>
@@ -1649,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.5" customHeight="1">
+    <row r="21" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -1673,7 +1678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="31.5" customHeight="1">
+    <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>21</v>
       </c>
@@ -1697,7 +1702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="29">
         <v>22</v>
       </c>
@@ -1721,7 +1726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1">
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <v>23</v>
       </c>
@@ -1745,7 +1750,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
         <v>24</v>
       </c>
@@ -1769,7 +1774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30.75" customHeight="1">
+    <row r="26" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <v>25</v>
       </c>
@@ -1793,7 +1798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="29">
         <v>26</v>
       </c>
@@ -1817,7 +1822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>27</v>
       </c>
@@ -1841,7 +1846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="46.5" customHeight="1">
+    <row r="29" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="29">
         <v>28</v>
       </c>
@@ -1865,7 +1870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="36" customHeight="1">
+    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>29</v>
       </c>
@@ -1918,13 +1923,13 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="141.1640625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="141.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="22" thickTop="1" thickBot="1">
+    <row r="1" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -1932,7 +1937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="21" thickBot="1">
+    <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
@@ -1940,7 +1945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="21" thickBot="1">
+    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -1948,7 +1953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="21" thickBot="1">
+    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
@@ -1956,7 +1961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" thickTop="1"/>
+    <row r="5" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
updated the bug matrix after filing issues
</commit_message>
<xml_diff>
--- a/metrics/bm.xlsx
+++ b/metrics/bm.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boyofthefuture\Documents\NetBeansProjects\is203_g3t3\metrics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="11835" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
     <sheet name="Guidelines" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
   <si>
     <t>Function</t>
   </si>
@@ -326,6 +321,12 @@
   </si>
   <si>
     <t>Top-K Dates</t>
+  </si>
+  <si>
+    <t>Top k Values</t>
+  </si>
+  <si>
+    <t>Top-k Does not account for the last record before midnight properly or there could be some logic issues</t>
   </si>
 </sst>
 </file>
@@ -1199,24 +1200,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="55.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1244,7 +1245,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23">
         <v>1</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -1346,7 +1347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -1373,7 +1374,7 @@
       <c r="H5" s="13"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -1402,13 +1403,13 @@
       </c>
       <c r="I6" s="14">
         <f>SUM(E:E)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="61" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33">
         <v>7</v>
       </c>
@@ -1458,7 +1459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="42.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33">
         <v>8</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="65.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="65.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>9</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
         <v>10</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>11</v>
       </c>
@@ -1558,7 +1559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33">
         <v>12</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33">
         <v>13</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>14</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>15</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
         <v>16</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
         <v>17</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
         <v>18</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>19</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -1775,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>21</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>22</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>23</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>24</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>25</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>26</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>27</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>28</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>29</v>
       </c>
@@ -1991,7 +1992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>30</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>31</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>32</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="29">
         <v>33</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="29">
         <v>34</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>35</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>36</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>37</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>38</v>
       </c>
@@ -2207,7 +2208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>39</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>40</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>41</v>
       </c>
@@ -2276,6 +2277,29 @@
         <v>98</v>
       </c>
       <c r="G42" s="47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="29">
+        <v>42</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="45">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" s="47" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2304,17 +2328,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="141.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" customWidth="1"/>
+    <col min="2" max="2" width="141.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -2322,7 +2346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
@@ -2330,7 +2354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -2338,7 +2362,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="20.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>28</v>
       </c>
@@ -2346,7 +2370,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:2" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>